<commit_message>
Update excel file, minor changes
</commit_message>
<xml_diff>
--- a/excel/Goniometer Angles to Dip, Azimuth.xlsx
+++ b/excel/Goniometer Angles to Dip, Azimuth.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Core basis vectors relative to " sheetId="1" state="visible" r:id="rId2"/>
@@ -42,6 +42,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Core direction vector </t>
     </r>
@@ -51,6 +52,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">d</t>
     </r>
@@ -62,6 +64,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">b = z</t>
     </r>
@@ -70,6 +73,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> x </t>
     </r>
@@ -79,6 +83,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">d</t>
     </r>
@@ -89,6 +94,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">| </t>
     </r>
@@ -98,6 +104,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">z</t>
     </r>
@@ -106,6 +113,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> x </t>
     </r>
@@ -115,6 +123,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">d</t>
     </r>
@@ -123,6 +132,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> |</t>
     </r>
@@ -136,6 +146,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Perpendicular vector </t>
     </r>
@@ -145,6 +156,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">s</t>
     </r>
@@ -155,6 +167,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Reference line vector </t>
     </r>
@@ -164,6 +177,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">r</t>
     </r>
@@ -234,6 +248,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Normal vector </t>
     </r>
@@ -243,6 +258,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">n </t>
     </r>
@@ -251,6 +267,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">relative to</t>
     </r>
@@ -260,6 +277,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> {d,r,s}</t>
     </r>
@@ -282,6 +300,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Normal vector </t>
     </r>
@@ -291,6 +310,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">n </t>
     </r>
@@ -299,6 +319,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">relative to</t>
     </r>
@@ -308,6 +329,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> {x,y,z}</t>
     </r>
@@ -340,6 +362,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -361,6 +384,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -423,20 +447,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,12 +476,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -531,16 +563,16 @@
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
+      <selection pane="bottomLeft" activeCell="P5" activeCellId="0" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,10 +621,10 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -821,12 +853,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -948,10 +980,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1050,7 +1082,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1065,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0</v>
@@ -1074,20 +1106,20 @@
         <v>0</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0</v>
+        <v>-0.841470984807896</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0</v>
+        <v>0.291926581726429</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0</v>
+        <v>0.454648713412841</v>
       </c>
       <c r="M5" s="0" t="n">
         <f aca="false">A5*$J5 + D5*$K5 + G5*$L5</f>
-        <v>0</v>
+        <v>-0.841470984807896</v>
       </c>
       <c r="N5" s="0" t="n">
         <f aca="false">B5*$J5 + E5*$K5 + H5*$L5</f>
@@ -1095,7 +1127,7 @@
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">C5*$J5 + F5*$K5 + I5*$L5</f>
-        <v>0</v>
+        <v>0.74657529513927</v>
       </c>
     </row>
   </sheetData>
@@ -1125,18 +1157,18 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.91"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1179,21 +1211,21 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>1</v>
+        <v>-0.841470984807896</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0</v>
+        <v>0.74657529513927</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">ACOS($C5)</f>
-        <v>1.5707963267949</v>
+        <v>0.727896827457617</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">ATAN2(B5, A5)</f>
-        <v>1.5707963267949</v>
+        <v>-1.5707963267949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>